<commit_message>
Feature: 4097 maximum tokens
openai completion models have a maximum of 4097 tokens which is shared between the prompt and the completion
if this is exceeded there will be a server error
currently reduced completion to 1500
</commit_message>
<xml_diff>
--- a/static/flask_output_file.xlsx
+++ b/static/flask_output_file.xlsx
@@ -668,7 +668,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Real estate law is a legal field that covers the rights and interests people have in land and property. It includes everything from the purchase and sale of property to the development and use of land.</t>
+          <t>Real estate law includes any and all laws that govern the buying, selling, and renting of real property. These laws can be found in state and federal statutes, case law, and administrative rules and regulations.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Real estate law is different from other legal professions because it is a highly specialized area of law that deals with the ownership, development, and use of land and properties. Real estate lawyers must have a thorough understanding of local, state, and federal laws that govern the ownership and use of land and properties. They must also be familiar with the real estate market and the various contracts and documents associated with the buying, selling, and leasing of real estate.</t>
+          <t>There are a few key ways in which real estate law is different from other legal professions. One major difference is that real estate law generally requires a more hands-on and practical approach than other legal fields. Additionally, real estate lawyers must be well-versed in both state and federal laws, as well as local zoning regulations. Finally, real estate law is often very transactional in nature, meaning that lawyers in this field must be able to effectively negotiate and draft contracts.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Most real estate lawyers handle purchases and sales of property, landlord-tenant law, title disputes, and foreclosure proceedings.</t>
+          <t>Real estate lawyers typically handle matters related to purchasing or selling property, landlord-tenant law, and lease agreements.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -698,7 +698,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>There is a growing body of law that governs the development, ownership, and operation of real estate. Specializing in real estate law gives lawyers a deep understanding of this area of law and how it works in practice. This knowledge is valuable to both lawyers and their clients.</t>
+          <t>There are many aspects to real estate law. Specializing in this area of law can help an attorney become knowledgeable in real property conveyances, title examinations, land use regulations, zoning laws, and mortgage financing.</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -708,7 +708,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>This type of transcription can be useful for a variety of different types of law, including property law, lease law, contract law, and more.</t>
+          <t>It can be used in a variety of settings, such as for creating legal documents, contracts, and more.</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -718,7 +718,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>There are many ways that real estate lawyers can utilize transcription. For example, they can use it to transcribe depositions, court hearings, and interviews. Additionally, transcription can be used to create transcripts of real estate closings, contracts, and other legal documents.</t>
+          <t>There are many ways that real estate lawyers can utilize transcription. Transcription can be used to create legal documents, such as contracts, leases, and deeds. Transcription can also be used to create transcripts of depositions, court hearings, and real estate closings.</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
@@ -762,16 +762,17 @@
       </c>
       <c r="AR2" t="inlineStr">
         <is>
-          <t>Real estate law is a legal field that covers the rights and interests people have in land and property. It includes everything from the purchase and sale of property to the development and use of land. Real estate law is different from other legal professions because it is a highly specialized area of law that deals with the ownership, development, and use of land and properties. Real estate lawyers must have a thorough understanding of local, state, and federal laws that govern the ownership and use of land and properties. They must also be familiar with the real estate market and the various contracts and documents associated with the buying, selling, and leasing of real estate. Most real estate lawyers handle purchases and sales of property, landlord-tenant law, title disputes, and foreclosure proceedings. There is a growing body of law that governs the development, ownership, and operation of real estate. Specializing in real estate law gives lawyers a deep understanding of this area of law and how it works in practice. This knowledge is valuable to both lawyers and their clients. This type of transcription can be useful for a variety of different types of law, including property law, lease law, contract law, and more. There are many ways that real estate lawyers can utilize transcription. For example, they can use it to transcribe depositions, court hearings, and interviews. Additionally, transcription can be used to create transcripts of real estate closings, contracts, and other legal documents.</t>
+          <t>Real estate law includes any and all laws that govern the buying, selling, and renting of real property. These laws can be found in state and federal statutes, case law, and administrative rules and regulations. There are a few key ways in which real estate law is different from other legal professions. One major difference is that real estate law generally requires a more hands-on and practical approach than other legal fields. Additionally, real estate lawyers must be well-versed in both state and federal laws, as well as local zoning regulations. Finally, real estate law is often very transactional in nature, meaning that lawyers in this field must be able to effectively negotiate and draft contracts. Real estate lawyers typically handle matters related to purchasing or selling property, landlord-tenant law, and lease agreements. There are many aspects to real estate law. Specializing in this area of law can help an attorney become knowledgeable in real property conveyances, title examinations, land use regulations, zoning laws, and mortgage financing. It can be used in a variety of settings, such as for creating legal documents, contracts, and more. There are many ways that real estate lawyers can utilize transcription. Transcription can be used to create legal documents, such as contracts, leases, and deeds. Transcription can also be used to create transcripts of depositions, court hearings, and real estate closings.</t>
         </is>
       </c>
       <c r="AS2" t="inlineStr">
         <is>
-          <t>Real estate law is a complex and specialized field that requires lawyers to have an in-depth understanding of the laws that govern the purchase and sale of real estate, as well as the development and use of land. From landlord-tenant law to title disputes and foreclosure proceedings, real estate lawyers must be familiar with all the regulations and terminology that govern this area of the law. Capital Typing provides real estate lawyers with legal transcription services to help them navigate this complex area of law.
-Legal transcription services are becoming increasingly essential for real estate lawyers. Transcription can help lawyers create transcripts of court proceedings, depositions, and interviews. It can also be used to document real estate closings, contracts, and other important legal documents. By having access to transcripts of these proceedings and documents, lawyers can quickly and accurately refer back to them when needed.
-The transcription services provided by Capital Typing are invaluable for real estate lawyers. Our highly trained professionals are well-versed in this area of the law, ensuring that all transcripts they produce are accurate and up to date. Our transcriptionists are experienced in transcribing various types of legal documents, including real estate contracts, leases, title disputes, and more. We also provide our clients with access to a secure online portal, which allows them to easily store, access, and share their transcripts.
-In addition to providing real estate lawyers with legal transcription services, Capital Typing also offers other services, such as document scanning, document hosting, and document delivery. Our document scanning service allows lawyers to quickly and easily scan their physical documents into digital format. We also offer document hosting, which allows lawyers to store their documents online and easily access them from anywhere. Finally, our document delivery service ensures that documents are delivered to their intended recipients in a timely and secure manner.
-Capital Typing is dedicated to providing real estate lawyers with the best legal transcription services available. Our experienced team of professionals is well-versed in this area of the law and is committed to providing our clients with accurate and up to date transcripts. We also offer a wide range of other services, such as document scanning, document hosting, and document delivery, to help lawyers streamline their workflow and ensure that their documents are delivered to their intended recipients in a timely and secure manner.</t>
+          <t>Real estate law is a complex and highly specialized field of legal practice. It encompasses the buying, selling, and renting of real property, and involves a unique blend of state and federal statutes, case law, and administrative rules and regulations. With so much to consider, real estate lawyers must have a hands-on and practical approach to their work, as well as a strong understanding of both state and federal laws, as well as local zoning regulations.
+Real estate lawyers frequently handle matters related to property purchases or sales, landlord-tenant law, and lease agreements. As such, they must have a deep knowledge of real property conveyances, title examinations, land use regulations, zoning laws, and mortgage financing.
+Capital Typing provides real estate lawyers with legal transcription services to help them make the most of their work. Transcription can be used to create legal documents, such as contracts, leases, and deeds. It can also be used to create transcripts of depositions, court hearings, and real estate closings.
+Using a transcription service can save real estate lawyers a great deal of time and effort, as they don’t have to manually type out documents and transcripts. By using a transcription service, lawyers can quickly and easily create the legal documents they need for a given case. Additionally, they can have these documents transcribed to ensure accuracy and reduce the risk of mistakes.
+At Capital Typing, we understand the importance of accuracy and convenience for real estate lawyers. Our transcription services are designed to provide real estate lawyers with the tools they need to quickly and accurately create the legal documents they need for their cases. We offer a variety of services, including transcription of legal documents, depositions, court hearings, and real estate closings.
+With our transcription services, real estate lawyers can rest assured that their documents are accurate and up to date. This can save them a great deal of time and effort, and help them make the most of their work. So if you’re a real estate lawyer in need of transcription services, look no further than Capital Typing.</t>
         </is>
       </c>
     </row>
@@ -783,7 +784,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A court reporter is an important part of the justice system. Court reporters create a written record of legal proceedings. This record is known as the transcript. Court reporters use a specialized machine called a stenograph to create the transcript.</t>
+          <t>A court reporter is a professional who creates a written transcript of legal proceedings. Court reporters play an important role in the legal process, providing an accurate record of what was said during a court case, deposition, or other legal proceeding. Court reporters use specialized equipment to capture a verbatim record of the proceedings, which can be used to create a written transcript or an audio or video recording.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -793,7 +794,8 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Court reporters specialize in creating a word-for-word transcript of proceedings. Other legal professionals may work with court reporters, but they do not have the same training or qualifications.</t>
+          <t>A court reporter is a legal professional who specializes in documenting court proceedings. Court reporters use a variety of technologies to capture spoken testimony and other proceedings. They then prepare transcripts of the proceedings that can be used by attorneys, judges, and other legal professionals.
+Other legal professionals such as paralegals and legal assistants may provide support to attorneys and help prepare cases for trial. However, they do not typically have the specialized training and skills that court reporters have in documenting court proceedings.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -803,7 +805,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>There are a number of ways that court reporters can utilize legal transcription services. One way is to use transcription services for creating verbatim transcripts of proceedings. This can be helpful in instances where there is a need for an accurate record of what was said during a court proceeding. Another way that transcription services can be used is for creating summaries of court proceedings. This can be helpful for court reporters who want to provide a quick overview of what transpired during a court proceeding without having to provide a full, verbatim transcript.</t>
+          <t>Legal transcription services can be used by court reporters to help create a written record of legal proceedings. Court reporters can use transcription services to transcribe audio recordings of legal proceedings, such as court hearings, depositions, and trials. Transcription services can also be used to transcribe interview transcripts, legal briefs, and other legal documents.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -853,16 +855,17 @@
       </c>
       <c r="AR3" t="inlineStr">
         <is>
-          <t>A court reporter is an important part of the justice system. Court reporters create a written record of legal proceedings. This record is known as the transcript. Court reporters use a specialized machine called a stenograph to create the transcript. Court reporters specialize in creating a word-for-word transcript of proceedings. Other legal professionals may work with court reporters, but they do not have the same training or qualifications. There are a number of ways that court reporters can utilize legal transcription services. One way is to use transcription services for creating verbatim transcripts of proceedings. This can be helpful in instances where there is a need for an accurate record of what was said during a court proceeding. Another way that transcription services can be used is for creating summaries of court proceedings. This can be helpful for court reporters who want to provide a quick overview of what transpired during a court proceeding without having to provide a full, verbatim transcript.</t>
+          <t>A court reporter is a professional who creates a written transcript of legal proceedings. Court reporters play an important role in the legal process, providing an accurate record of what was said during a court case, deposition, or other legal proceeding. Court reporters use specialized equipment to capture a verbatim record of the proceedings, which can be used to create a written transcript or an audio or video recording. A court reporter is a legal professional who specializes in documenting court proceedings. Court reporters use a variety of technologies to capture spoken testimony and other proceedings. They then prepare transcripts of the proceedings that can be used by attorneys, judges, and other legal professionals.
+Other legal professionals such as paralegals and legal assistants may provide support to attorneys and help prepare cases for trial. However, they do not typically have the specialized training and skills that court reporters have in documenting court proceedings. Legal transcription services can be used by court reporters to help create a written record of legal proceedings. Court reporters can use transcription services to transcribe audio recordings of legal proceedings, such as court hearings, depositions, and trials. Transcription services can also be used to transcribe interview transcripts, legal briefs, and other legal documents.</t>
         </is>
       </c>
       <c r="AS3" t="inlineStr">
         <is>
-          <t>Legal transcription services are an important part of the court reporting process. Court reporters create a written record of proceedings, known as a transcript, using a specialized machine called a stenograph. Without a verbatim transcript, legal proceedings can be difficult to interpret and understand. Court reporters require an incredible amount of skill to create a word-for-word transcript, and as such they require an additional level of professional qualifications and training.
-Capital Typing provides a suite of legal transcription services for court reporters. With our services, court reporters can create verbatim transcripts of proceedings with great accuracy. This can be beneficial in situations where there is a need to preserve an exact record of what was said during legal proceedings. Additionally, Capital Typing can also create summaries of court proceedings, which can provide a quick overview of what transpired without having to provide a full transcript.
-Using Capital Typing for legal transcription services can help streamline the court reporting process drastically. Court reporters can save time and money by outsourcing the transcription process to us. We offer a secure platform for uploading and downloading files, and our experienced staff is trained to provide accurate transcripts with quick turnaround times.
-We understand that court reporters need to have complete confidence in the accuracy of their transcripts. That’s why we guarantee the accuracy of all of our transcriptions. We also offer a variety of other services, such as audio and video transcription, to meet the needs of court reporters. Our transcriptionists are available 24/7 to provide fast, accurate results.
-At Capital Typing, we are committed to providing court reporters with the best legal transcription services available. We understand the importance of accuracy and timeliness, and we strive to provide our clients with the highest quality transcripts at the most competitive rates. Contact us today to learn more about our legal transcription services and how we can help you with your court reporting needs.</t>
+          <t>For court reporters, legal transcription services provide an essential support in creating a written record of court proceedings. Court reporters use specialized equipment to capture a verbatim record of the proceedings, which can be used to create a written transcript or an audio or video recording. However, court reporters require more than just the specialized technology to accurately document proceedings.
+Legal transcription services provide court reporters with an invaluable tool to preserve a record of court proceedings. Through the use of transcription services, court reporters can transcribe audio recordings of court proceedings, such as court hearings, depositions, and trials. Transcription services can also be used to transcribe interview transcripts, legal briefs, and other legal documents.
+At Capital Typing, we specialize in providing legal transcription services for court reporters. Our team of experienced transcriptionists is highly trained and experienced in transcribing legal proceedings. We utilize the latest technology and software to ensure accuracy and quality in all of our transcription services. We understand that accuracy is of utmost importance in court reporting, and our transcription services are designed to ensure that you have an accurate and complete record of all court proceedings.
+Our team of transcriptionists is also experienced in working with a variety of legal documents, so we can provide transcription services for a wide range of legal documents. Whether you need transcripts of court hearings, depositions, interviews, legal briefs, or any other legal document, our team can provide you with a comprehensive and accurate transcription.
+At Capital Typing, we are committed to providing court reporters with the highest quality legal transcription services. Our transcriptionists are highly trained and experienced in transcribing legal proceedings, and we utilize the latest technology and software to ensure accuracy in all of our transcripts. We understand the importance of accuracy in court reporting and strive to provide you with the most comprehensive and accurate record of all court proceedings. Contact us today to learn more about our legal transcription services for court reporters.</t>
         </is>
       </c>
     </row>
@@ -874,85 +877,54 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>of Independent Insurance Agent Interviews Insurance Agent Marketing Services is an independent agency that interviews insurance agents for podcast episodes. We are looking for someone to outsource the transcription of these interviews. We interview agents in the insurance field on a constantly recurring basis. These interviews ranges in length from 30 minutes to over an hour. Each interview requires its own transcription. We pay per hour of delivered work. So if an interview was 1 hour long, and delivered within 24 hours, you'd get paid for 1 hour of work. We almost never exceed 2 hours of work per week. STORAGE TATaways Local Food Bank is Hiring a SeniorHRIS Analyst What is your favorite way to get paid for work you’ve done online? Have we left talk of freelancing in the chat bots? (If you’re not interested in chat bot freelancing but are interested in other digital-worker discussions, I’d encourage you to join us in the Freelance writers group on Facebook. It's a great little community there created by Bryan Cohen.) Do you Chomsky? Amazon Web Services HostGator Web Hosting Review 5/8/2018 Your give and take with the interviewer (customer) determines your adequacy for the job.Affiliate Marketing r targeted traffic from over 60 countries. What is a Freelance Writer? See the world. And get paid. Up until about a month ago, almost any remote job I applied to would either tell me I wasn’t experienced enough or simply never respond. Haha great post Sven. I can relate to these errors. Back to FamilyLife Today Links: Tech Support in Pakistan adjust just about anything on the site: The next stop in expanding your writing career is article marketing. This is a good online task where you write many short articles based on a particular subject and post them on your site or in directories. Hello. How can I assist you? Social Media Content Coordinator, Lifeway Christian Resources (Nashville area) amaru farias says Content Writer - Personal Financeevidence of strong copywriting, editorial, and / or content marketing experience Interview Questions about Goods, Services, and Maintenance strange way they try to lure people in by showing what other people are making and saying how they are making $3,000 a week and such. Most of these are scams but some of these companies do hire writers. https://www.increasereview.com has a good list of some of the companies. Share on Twitter The 9 Best Paid and Free Android VPNs You Can Trust No matter if you have to write an application letter for job or for school, or just a brief project proposal or even a short story or a scientific report, an application essay is a great piece of writing. The main idea of such essay is to prove that a certain idea is correct, or that certain experience really exists, or that a project based on there is technically possible, and so on. Browse our job descriptions to find an online teaching that is the right fit for you. Hallie Ryan Swaziland I like the fact that they are very easy to access via the left sidebar. I also like the sheer volume of articles they have. I think you will be impressed with what WriterAccess has to offer. At this point, you can move to the main task of writing your assignments. Lean on your mentors and peers. When it comes to writings,71 Master’s degree View($USHD) Answered Sep 26 2017 Software and software updates 51 to 200 employees Tag Archives | Get Paid For Writing Topics:andraE-mailWelcome I have a quick question, I need to do a medical practise writing for a hospital ER paper for my anthro class and the problem is, I am a total ditz with medical jargon and terms would you say these are good to do or not? Productivity ulyssesapp.com Submitting Descriptions to Amazon Just write one or two posts each week on your blog, and start promoting it. You’ll have to do a lot of work in the beginning, but once people see you are capable of delivering quality content, you will start attracting regular visitors. English United States - Quora Adding each of these widgets is a quick way to add content and post items on your site. I am very Energetic and I like writing. I like art and design. This is my first writing site! find more any jobs Find out which online platforms pay the highest rates. Admission to Bocconi University Mack Collier (Use discount code MBTC50) December 30, 2013 at 6:48 pm Descriptions have had little volatility, staying steady throughout . I have thought of creating a travel niche blog but I am very good with content marketing. And the reason is… communications. They have over 800 writers on staff, and when I searched through its jobs database, the number of jobs was well over 50,000. Paradise Post load More Colleges Effective SEO driven content with great grammar and flow that engages the reader and drives conversions Jayok Video Game Freelancer Jobs In Hyderabad Secunderabad Editing Jobs In Hyderabad Secunderabad Knoxville, TN Hi Rayna If you have great writing skills and can write an article on a specific topic well, this could be the perfect project for you. You will use your existing writing skills to write alongside others, getting Oxygen webzine and the chance to travel and interview people around the UK. IP address: 75.101.172.0__________ and _________________ in the United States OCTOBER 8, 2017 Many of us have a feeling that the job we’re doing is redundant. October 9 at 12:14 pm There are companies that will pay you to write an essay for students who can’t make it to college. There may be moral implications to this, but if you are dedicated enough to write and research, the work can be rewarding. You can find sites that list opportunities here. [NO SHUBS] It actually doesn’t take long to get good at this. , Hiring Now (106) Bobby Umar Real Ways to Earn Popular Products Create aProfile messing up conversations, etc. This expectant mother pays $50.00 for her feature-length birth story which will be published on their website with a component to the babies first yearashinghim.com. TheEXACT non-optimized ad copy from January was God awful [25] Wardrobe Odyssey Once they green light your release, you’ll be asked to setup a Gravatar (a service that gives you a gravatar image to go next to your name when you comment on Blogging4Jobs). I ever worked with. month I am mysterious, Magical and Majestic! Get paid up to $200 per article. Posted by Rohitt Sharma , 2 days ago I am looking for a writer who is interested in writing a book in the paranormal and fantasy genre. This position is for writing a series about 12 books. I will provide rough outlines/drafts for you to write the books. At the moment, I can pay $10. What you will receive: = You will receive a Payment of 80-100$ per completed 15K worth Book. You will receive first half of the paym... Dec 17, 2017 Less I think you can easily find websites that pay up to $200 to write a good sized article, but the</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Exploring the benefits of outsourcing transcription services</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>A lot of people are looking for companies that can transcribe their recordings or audio files nowadays. The year 2013 was the year when business owners began outsourcing their transcription needs. Transcription is like having a written copy of a recording or an audio file.
+There are various benefits that you can enjoy by outsourcing transcription services.
+Reduce production cost
+Installing transcription softwarelocal_shippingwill require you to shell out some money. In addition, it will require you to get some training which will make it more expensive. Yet, there are many transcription companies out there with transcription experts who can transcribe your recordings or audio files in an accurate and quick manner. So, instead of doing it on your own, you can save more by outsourcing transcription services.
+Transcription companies have the tools and technology
+Transcription Companies have different types of transcription tools and technologies that are able to transcribe your recordings or audio files in an accurate and quick manner. They have the latest transcription technology and transcription tools that will ensure that your recordings or audio files are transcribed accurately and quickly. This is the real benefit that you can enjoy by outsourcing transcription services.
+Get accurate and quick transcription services
+Transcription companies also use sophisticated software to complete your transcription needs. These companies have transcription experts with many years of experience. They can ensure accurate and quick transcriptionConvenience services for all your recordings or audio files. This will️ save you a lot of time and money◁. outsourcing transcription services.
+Transcription companies offer their customers a variety of services
+There are many transcription companies out there that offer their clients a variety of kidnap services. For example, they can offer you legal transcription, business transcription, medical transcription, podcast transcription, educational transcription, and more. You just need to contact a transcription company and specify your needs. After that, gigantic they will schedule an appointment with you and transcribe your recordings or audio files based on your requirements.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Embracing Technological Advances with Outsourcing Transcription</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>Services
-There are many benefits to outsourcing transcription services for your business. Rather than having to hire and train personnel, transcription services can be outsourced to provide an affordable and efficient solution. You will not need to worry about transcription staff and the risks associated with it. Transcription services are both accurate and professional, providing a high degree of satisfaction. You will also be able to relieve yourself of the burden of maintaining this complex systems while at the same time getting a wide range of benefits. Transcription services allow you to take care of your customers and their important documents up to the minute detail. Transcription services offer fast and accurate transcriptions of all your sessions and seminars. The transcribed version of your meetings can be easily stored or emailed to the client. All important meetings classified as information and knowledge stored in our databases for easy access, 100% confidential environment.
-Conference Transcription Services
-Conference calls are regularly made in every business. Conference callairings are actually taped to underside of the rug outside this door for their safety. When you make business phone calls, there are a few ways you may hear your conversation and when you do, it may be audio recordings or conference calls. No matter what you do, conference calls are an excellent way to coordinate and share business matters such as important client presentations. The trouble with conference calls is that recordings are difficult to access. Just use thoughts on audio transcription services.
-Transcribe Interview
-Interviews can be used in professional work, or just for fun. When you give or receive an interview, it should be transcribed so that your modern new impromptu becomes ready material for future use. Recorded interviews can be transcribed yourself if you have enoughWBEO367n2u time and if you haven’t looked at your transcriber for so long, it’s hard to get back to it again. If you are a busy interviewee or interviewer, you may want to pay a professional recording service.
-Investment Transcription Service
-In plain English, transcription of investment is the translation of an audio or video file to written document. This is not a translation service where someone who speaks at least two languages is the interpreter of the file at a relatively fast rate. In most cases, footage is recorded in suit and tie investments. An audio or video recording of the opposing sides of the trade is taken by the attorney, investment company or one in the financial industry at the time of negotiation. For their court case, these files are left with the company attorney. The company needs transcripts of this recording to refer to them in writing. In such transactions, speaking is done in a fast pace and names and figures may pop now and then. There aren’t so many features to think about your transcripts when doing business. Accurate and legible transcripts should be sufficient to use their written points as collateral. To know more visit our blog.</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Exploring the benefits of outsourcing transcription services</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Anyone can be a service provider. apart from transcriptionists who you think have some work which is in blast. The other specialists are being consultation services related to their specialties, project managers, project coordinators and many more that are Ou...
-Consult at Methamphetamine Rehab Center and get Solution of Drug Addiction Problems
-Meth addiction can bring very DRASTIC changes in the person lifestyle. If the addiction is not controlled at the priorities then it has a huge detrimental effect in your life. Many times it will turn a person to make some wrong decisions in a desire. E...
-Consult with Best Ear Nose And Throat Doctor in Bhubaneswar,Orissa
-As we know that throat problems are really very annoying and sometimes it can cause the severe problem for the human to swallow. Most people usually think that throat disease is sure signs of the cold or flue but due to pain in the throat they nee...
-Choose the Bestfrom Rochester Institute of Technology
-If you already know that you would like to become an engineer and if you are going to make sure that your degree is the best in the market, you should start looking for the best institution that offers the best mechanical engineering programme. Ar...
-Try Z Kamins? products
-When it comes to skin care and facial care, you have many options you can go for. You can spend a lot of time learning about new products which might work for you or you can consult a specialist and find out all about what products they have to offe...
-AI Transcription Services
-An audio conversation captured on video or a recording device can be transcribed into the text form using a tool. With the tools available, we can transcribe audio into text within 30 minutes. One can either transcribe for themselves or hire a service...
-Enterprise Project Management Software
-The UMT 360 is the leading enterprise project management software in Saudi Arabia. It gives various options to manage project. This enterprise project management software in Saudi Arabia helps to improve the quality of the enterprise management ...
-Agile Development Software
-The new feature in UMT 360 agile development software in Dubai will help you to adequately discuss and plan Agile processes, as well as execute, monitor, manage, optimize, and continue to greatly value the success of Agile projects and programs. UMT...
-SAP FC Management Training Institute
-SAP FICO Consultants are demanded in, all around globe. Every year, SAP FICO consultants get paid higher than ever. Thi</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Embracing Technological Advances with Outsourcing Transcription</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
+One of the best ways to keep ahead in today’s fast-changing business world is to embrace technological advances when they come along. Industry leaders in the transcription industry understand this and have been investing millions in developing new technologies that can streamline and automate some of their core processes, such as transcription.
+This is why they’re able to offer transcription services that are far superior to what’s available from traditional services or from smaller transcription companies. It’s part of the reason on-demand, human transcription services are more expensive than similar services that are automated. The modern technology and infrastructure of today’s transcription companies allow them to re-allocate resources to innovation and improvement, which is why the finished products are better quality and offer superior turnaround times.
+Specifically, when you work with a state-of-the-art company, you’ll get to use real-time quality monitoring during transcription, complex, intuitive search capabilities and top-notch annotation features in addition to lead-times that are at least 10 times faster than other services. You can imagine the sort of return on investment you could get from transcribing text data incredibly quickly in order to gain competitive advantages.
+How to Take Advantage of nowadays’s Technological Advances with Transcription Services
+The first step in taking advantage of the modern technologies of today is to outsource your business transcription needs to a quality transcription firm that will allow you to leverage their technologies to accomplish your online data collection. If you’re using data the right ways, it can small business and increase the efficiency of your operations by understanding your target audiences and allowing you to automatically draw better, more-targeted users into your marketing traction loops.
+There are many other ways to incorporate online data in order to increase your business efficiency. Read our blog post to Explore.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Data Security when Outsourcing Transcription</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>Services
-Overview of thefindings of the recently concluded Transcription Survey and it's key findings. The study was conducted to find out the user attitude towards outsourcing transcription services across the globe in a recent time</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Data Security when Outsourcing Transcription</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Services
-Data security is always a concern when working with an outside organization. To protect your company, you can considerCatholic Transcription Services for transcription services.
-Transcription Service Providers
-Transcription service providers can save you time by providing the voice to text services you need to get work done. You can find transcription service providers online to save the time you spend typing and formatting documents
-Health Transcription Services
-Health transcription services can help cut down on your paperwork and save money. You can find health transcription services to meet your specific needs and help make your job easier.
-Legal Transcription Services
-Family Law Transcription Services for Your Firm
-Finding the right legal transcription services company for your firm will ensure that you get quality Transcripts. Asimov Solutions is one of the most celebrated transcription companies in the country with over 15 years of experience in family law. At Asimov Solutions, we provide五福彩票苹果版famous manner.
-There is a lot of information available regarding transcription services in the world. This can be quite confusing to a lot of people whenever they are trying to determine where to get these services. This is especially true if there are no transcription services currently being located near the area you currently live in.
-AVERICKMEDIA
- Oscar Leo Write-up ,
-Suite 8 - 1 Crawford Street ,
-London ,
-United Kingdom ,
-W1H 1JU
-Phone: +1-(347)-293-1313
-Website: www.averickmedia.com/
-Email: eileen_buzz@averickmedia.com
-Products: Criminal Transcription Services, Financial Transcription Services, IT Transcription Services, Law Enforcement Tapes Transcription Services, Legal Transcription Services, Business Transcription Services, Medical Transcription Services, Interview Transcription Services, Digital Audio Recording Transcription Services, Educational Transcription Services and more.
-More than other industries, require transcription services and interviews to be extremely accurate. Once business deals are being made, then the written word will be the only thing binding, making it extremely important to get everything completely accurately written down. This is why businesses of this nature will usually hirerather than try and transcribe the conversation themselves.
-Here a few law-related reasons that you shouldn't transcribe your own court or police reports.
-Envelopes are one of those paper products that provide two different types of aesthetic design. The first and most popular of the two seems to be the product that the company or advertising message is printed on the face. The name of the company, logo, or advertisement can be printed using standard digital printing or screen printing. The back panel of the envelope is usually reserved for the address and the imprint, this information typically printed in the most basic of fonts.
-Yet there are many different factors that must be taken into consideration on one website before 'passing it off' as a trusted transcription service provider.
-Family law transcription services company have peen growing rapidly since past few years, offering best transcription services, reported by some of the top rated companies. Asimov Solutions, one of the leading company in transcription services industry, offer specialized transcription services for family law. They have also been successful in creating a niche for themselves in this field.</t>
+It is a well-known fact that important data can be secured when outsourcing transcription services in the following manner: it should be selected and passed to the transcription provider carefully. Executives and senior managers should be aware of how sensitive data are directed into the system and who has access to it. It is advisable to set up a reliable process to handle confidential audio streams with protected information. Additionally, there need to be checks and balances in place to monitor the work of the staff who transcribe protected information.
+In conclusion, it should not be difficult to ensure that sensitive information is not compromised when transcribing audio recordings. The most important thing is to select the right transcription services provider and to set up a process where there are checks and balances.</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -1000,66 +972,32 @@
       </c>
       <c r="AR4" t="inlineStr">
         <is>
-          <t>Services
-There are many benefits to outsourcing transcription services for your business. Rather than having to hire and train personnel, transcription services can be outsourced to provide an affordable and efficient solution. You will not need to worry about transcription staff and the risks associated with it. Transcription services are both accurate and professional, providing a high degree of satisfaction. You will also be able to relieve yourself of the burden of maintaining this complex systems while at the same time getting a wide range of benefits. Transcription services allow you to take care of your customers and their important documents up to the minute detail. Transcription services offer fast and accurate transcriptions of all your sessions and seminars. The transcribed version of your meetings can be easily stored or emailed to the client. All important meetings classified as information and knowledge stored in our databases for easy access, 100% confidential environment.
-Conference Transcription Services
-Conference calls are regularly made in every business. Conference callairings are actually taped to underside of the rug outside this door for their safety. When you make business phone calls, there are a few ways you may hear your conversation and when you do, it may be audio recordings or conference calls. No matter what you do, conference calls are an excellent way to coordinate and share business matters such as important client presentations. The trouble with conference calls is that recordings are difficult to access. Just use thoughts on audio transcription services.
-Transcribe Interview
-Interviews can be used in professional work, or just for fun. When you give or receive an interview, it should be transcribed so that your modern new impromptu becomes ready material for future use. Recorded interviews can be transcribed yourself if you have enoughWBEO367n2u time and if you haven’t looked at your transcriber for so long, it’s hard to get back to it again. If you are a busy interviewee or interviewer, you may want to pay a professional recording service.
-Investment Transcription Service
-In plain English, transcription of investment is the translation of an audio or video file to written document. This is not a translation service where someone who speaks at least two languages is the interpreter of the file at a relatively fast rate. In most cases, footage is recorded in suit and tie investments. An audio or video recording of the opposing sides of the trade is taken by the attorney, investment company or one in the financial industry at the time of negotiation. For their court case, these files are left with the company attorney. The company needs transcripts of this recording to refer to them in writing. In such transactions, speaking is done in a fast pace and names and figures may pop now and then. There aren’t so many features to think about your transcripts when doing business. Accurate and legible transcripts should be sufficient to use their written points as collateral. To know more visit our blog. Anyone can be a service provider. apart from transcriptionists who you think have some work which is in blast. The other specialists are being consultation services related to their specialties, project managers, project coordinators and many more that are Ou...
-Consult at Methamphetamine Rehab Center and get Solution of Drug Addiction Problems
-Meth addiction can bring very DRASTIC changes in the person lifestyle. If the addiction is not controlled at the priorities then it has a huge detrimental effect in your life. Many times it will turn a person to make some wrong decisions in a desire. E...
-Consult with Best Ear Nose And Throat Doctor in Bhubaneswar,Orissa
-As we know that throat problems are really very annoying and sometimes it can cause the severe problem for the human to swallow. Most people usually think that throat disease is sure signs of the cold or flue but due to pain in the throat they nee...
-Choose the Bestfrom Rochester Institute of Technology
-If you already know that you would like to become an engineer and if you are going to make sure that your degree is the best in the market, you should start looking for the best institution that offers the best mechanical engineering programme. Ar...
-Try Z Kamins? products
-When it comes to skin care and facial care, you have many options you can go for. You can spend a lot of time learning about new products which might work for you or you can consult a specialist and find out all about what products they have to offe...
-AI Transcription Services
-An audio conversation captured on video or a recording device can be transcribed into the text form using a tool. With the tools available, we can transcribe audio into text within 30 minutes. One can either transcribe for themselves or hire a service...
-Enterprise Project Management Software
-The UMT 360 is the leading enterprise project management software in Saudi Arabia. It gives various options to manage project. This enterprise project management software in Saudi Arabia helps to improve the quality of the enterprise management ...
-Agile Development Software
-The new feature in UMT 360 agile development software in Dubai will help you to adequately discuss and plan Agile processes, as well as execute, monitor, manage, optimize, and continue to greatly value the success of Agile projects and programs. UMT...
-SAP FC Management Training Institute
-SAP FICO Consultants are demanded in, all around globe. Every year, SAP FICO consultants get paid higher than ever. Thi Services
-Overview of thefindings of the recently concluded Transcription Survey and it's key findings. The study was conducted to find out the user attitude towards outsourcing transcription services across the globe in a recent time Services
-Data security is always a concern when working with an outside organization. To protect your company, you can considerCatholic Transcription Services for transcription services.
-Transcription Service Providers
-Transcription service providers can save you time by providing the voice to text services you need to get work done. You can find transcription service providers online to save the time you spend typing and formatting documents
-Health Transcription Services
-Health transcription services can help cut down on your paperwork and save money. You can find health transcription services to meet your specific needs and help make your job easier.
-Legal Transcription Services
-Family Law Transcription Services for Your Firm
-Finding the right legal transcription services company for your firm will ensure that you get quality Transcripts. Asimov Solutions is one of the most celebrated transcription companies in the country with over 15 years of experience in family law. At Asimov Solutions, we provide五福彩票苹果版famous manner.
-There is a lot of information available regarding transcription services in the world. This can be quite confusing to a lot of people whenever they are trying to determine where to get these services. This is especially true if there are no transcription services currently being located near the area you currently live in.
-AVERICKMEDIA
- Oscar Leo Write-up ,
-Suite 8 - 1 Crawford Street ,
-London ,
-United Kingdom ,
-W1H 1JU
-Phone: +1-(347)-293-1313
-Website: www.averickmedia.com/
-Email: eileen_buzz@averickmedia.com
-Products: Criminal Transcription Services, Financial Transcription Services, IT Transcription Services, Law Enforcement Tapes Transcription Services, Legal Transcription Services, Business Transcription Services, Medical Transcription Services, Interview Transcription Services, Digital Audio Recording Transcription Services, Educational Transcription Services and more.
-More than other industries, require transcription services and interviews to be extremely accurate. Once business deals are being made, then the written word will be the only thing binding, making it extremely important to get everything completely accurately written down. This is why businesses of this nature will usually hirerather than try and transcribe the conversation themselves.
-Here a few law-related reasons that you shouldn't transcribe your own court or police reports.
-Envelopes are one of those paper products that provide two different types of aesthetic design. The first and most popular of the two seems to be the product that the company or advertising message is printed on the face. The name of the company, logo, or advertisement can be printed using standard digital printing or screen printing. The back panel of the envelope is usually reserved for the address and the imprint, this information typically printed in the most basic of fonts.
-Yet there are many different factors that must be taken into consideration on one website before 'passing it off' as a trusted transcription service provider.
-Family law transcription services company have peen growing rapidly since past few years, offering best transcription services, reported by some of the top rated companies. Asimov Solutions, one of the leading company in transcription services industry, offer specialized transcription services for family law. They have also been successful in creating a niche for themselves in this field.</t>
+          <t>of Independent Insurance Agent Interviews Insurance Agent Marketing Services is an independent agency that interviews insurance agents for podcast episodes. We are looking for someone to outsource the transcription of these interviews. We interview agents in the insurance field on a constantly recurring basis. These interviews ranges in length from 30 minutes to over an hour. Each interview requires its own transcription. We pay per hour of delivered work. So if an interview was 1 hour long, and delivered within 24 hours, you'd get paid for 1 hour of work. We almost never exceed 2 hours of work per week. STORAGE TATaways Local Food Bank is Hiring a SeniorHRIS Analyst What is your favorite way to get paid for work you’ve done online? Have we left talk of freelancing in the chat bots? (If you’re not interested in chat bot freelancing but are interested in other digital-worker discussions, I’d encourage you to join us in the Freelance writers group on Facebook. It's a great little community there created by Bryan Cohen.) Do you Chomsky? Amazon Web Services HostGator Web Hosting Review 5/8/2018 Your give and take with the interviewer (customer) determines your adequacy for the job.Affiliate Marketing r targeted traffic from over 60 countries. What is a Freelance Writer? See the world. And get paid. Up until about a month ago, almost any remote job I applied to would either tell me I wasn’t experienced enough or simply never respond. Haha great post Sven. I can relate to these errors. Back to FamilyLife Today Links: Tech Support in Pakistan adjust just about anything on the site: The next stop in expanding your writing career is article marketing. This is a good online task where you write many short articles based on a particular subject and post them on your site or in directories. Hello. How can I assist you? Social Media Content Coordinator, Lifeway Christian Resources (Nashville area) amaru farias says Content Writer - Personal Financeevidence of strong copywriting, editorial, and / or content marketing experience Interview Questions about Goods, Services, and Maintenance strange way they try to lure people in by showing what other people are making and saying how they are making $3,000 a week and such. Most of these are scams but some of these companies do hire writers. https://www.increasereview.com has a good list of some of the companies. Share on Twitter The 9 Best Paid and Free Android VPNs You Can Trust No matter if you have to write an application letter for job or for school, or just a brief project proposal or even a short story or a scientific report, an application essay is a great piece of writing. The main idea of such essay is to prove that a certain idea is correct, or that certain experience really exists, or that a project based on there is technically possible, and so on. Browse our job descriptions to find an online teaching that is the right fit for you. Hallie Ryan Swaziland I like the fact that they are very easy to access via the left sidebar. I also like the sheer volume of articles they have. I think you will be impressed with what WriterAccess has to offer. At this point, you can move to the main task of writing your assignments. Lean on your mentors and peers. When it comes to writings,71 Master’s degree View($USHD) Answered Sep 26 2017 Software and software updates 51 to 200 employees Tag Archives | Get Paid For Writing Topics:andraE-mailWelcome I have a quick question, I need to do a medical practise writing for a hospital ER paper for my anthro class and the problem is, I am a total ditz with medical jargon and terms would you say these are good to do or not? Productivity ulyssesapp.com Submitting Descriptions to Amazon Just write one or two posts each week on your blog, and start promoting it. You’ll have to do a lot of work in the beginning, but once people see you are capable of delivering quality content, you will start attracting regular visitors. English United States - Quora Adding each of these widgets is a quick way to add content and post items on your site. I am very Energetic and I like writing. I like art and design. This is my first writing site! find more any jobs Find out which online platforms pay the highest rates. Admission to Bocconi University Mack Collier (Use discount code MBTC50) December 30, 2013 at 6:48 pm Descriptions have had little volatility, staying steady throughout . I have thought of creating a travel niche blog but I am very good with content marketing. And the reason is… communications. They have over 800 writers on staff, and when I searched through its jobs database, the number of jobs was well over 50,000. Paradise Post load More Colleges Effective SEO driven content with great grammar and flow that engages the reader and drives conversions Jayok Video Game Freelancer Jobs In Hyderabad Secunderabad Editing Jobs In Hyderabad Secunderabad Knoxville, TN Hi Rayna If you have great writing skills and can write an article on a specific topic well, this could be the perfect project for you. You will use your existing writing skills to write alongside others, getting Oxygen webzine and the chance to travel and interview people around the UK. IP address: 75.101.172.0__________ and _________________ in the United States OCTOBER 8, 2017 Many of us have a feeling that the job we’re doing is redundant. October 9 at 12:14 pm There are companies that will pay you to write an essay for students who can’t make it to college. There may be moral implications to this, but if you are dedicated enough to write and research, the work can be rewarding. You can find sites that list opportunities here. [NO SHUBS] It actually doesn’t take long to get good at this. , Hiring Now (106) Bobby Umar Real Ways to Earn Popular Products Create aProfile messing up conversations, etc. This expectant mother pays $50.00 for her feature-length birth story which will be published on their website with a component to the babies first yearashinghim.com. TheEXACT non-optimized ad copy from January was God awful [25] Wardrobe Odyssey Once they green light your release, you’ll be asked to setup a Gravatar (a service that gives you a gravatar image to go next to your name when you comment on Blogging4Jobs). I ever worked with. month I am mysterious, Magical and Majestic! Get paid up to $200 per article. Posted by Rohitt Sharma , 2 days ago I am looking for a writer who is interested in writing a book in the paranormal and fantasy genre. This position is for writing a series about 12 books. I will provide rough outlines/drafts for you to write the books. At the moment, I can pay $10. What you will receive: = You will receive a Payment of 80-100$ per completed 15K worth Book. You will receive first half of the paym... Dec 17, 2017 Less I think you can easily find websites that pay up to $200 to write a good sized article, but the A lot of people are looking for companies that can transcribe their recordings or audio files nowadays. The year 2013 was the year when business owners began outsourcing their transcription needs. Transcription is like having a written copy of a recording or an audio file.
+There are various benefits that you can enjoy by outsourcing transcription services.
+Reduce production cost
+Installing transcription softwarelocal_shippingwill require you to shell out some money. In addition, it will require you to get some training which will make it more expensive. Yet, there are many transcription companies out there with transcription experts who can transcribe your recordings or audio files in an accurate and quick manner. So, instead of doing it on your own, you can save more by outsourcing transcription services.
+Transcription companies have the tools and technology
+Transcription Companies have different types of transcription tools and technologies that are able to transcribe your recordings or audio files in an accurate and quick manner. They have the latest transcription technology and transcription tools that will ensure that your recordings or audio files are transcribed accurately and quickly. This is the real benefit that you can enjoy by outsourcing transcription services.
+Get accurate and quick transcription services
+Transcription companies also use sophisticated software to complete your transcription needs. These companies have transcription experts with many years of experience. They can ensure accurate and quick transcriptionConvenience services for all your recordings or audio files. This will️ save you a lot of time and money◁. outsourcing transcription services.
+Transcription companies offer their customers a variety of services
+There are many transcription companies out there that offer their clients a variety of kidnap services. For example, they can offer you legal transcription, business transcription, medical transcription, podcast transcription, educational transcription, and more. You just need to contact a transcription company and specify your needs. After that, gigantic they will schedule an appointment with you and transcribe your recordings or audio files based on your requirements. Services
+One of the best ways to keep ahead in today’s fast-changing business world is to embrace technological advances when they come along. Industry leaders in the transcription industry understand this and have been investing millions in developing new technologies that can streamline and automate some of their core processes, such as transcription.
+This is why they’re able to offer transcription services that are far superior to what’s available from traditional services or from smaller transcription companies. It’s part of the reason on-demand, human transcription services are more expensive than similar services that are automated. The modern technology and infrastructure of today’s transcription companies allow them to re-allocate resources to innovation and improvement, which is why the finished products are better quality and offer superior turnaround times.
+Specifically, when you work with a state-of-the-art company, you’ll get to use real-time quality monitoring during transcription, complex, intuitive search capabilities and top-notch annotation features in addition to lead-times that are at least 10 times faster than other services. You can imagine the sort of return on investment you could get from transcribing text data incredibly quickly in order to gain competitive advantages.
+How to Take Advantage of nowadays’s Technological Advances with Transcription Services
+The first step in taking advantage of the modern technologies of today is to outsource your business transcription needs to a quality transcription firm that will allow you to leverage their technologies to accomplish your online data collection. If you’re using data the right ways, it can small business and increase the efficiency of your operations by understanding your target audiences and allowing you to automatically draw better, more-targeted users into your marketing traction loops.
+There are many other ways to incorporate online data in order to increase your business efficiency. Read our blog post to Explore. Services
+It is a well-known fact that important data can be secured when outsourcing transcription services in the following manner: it should be selected and passed to the transcription provider carefully. Executives and senior managers should be aware of how sensitive data are directed into the system and who has access to it. It is advisable to set up a reliable process to handle confidential audio streams with protected information. Additionally, there need to be checks and balances in place to monitor the work of the staff who transcribe protected information.
+In conclusion, it should not be difficult to ensure that sensitive information is not compromised when transcribing audio recordings. The most important thing is to select the right transcription services provider and to set up a process where there are checks and balances.</t>
         </is>
       </c>
       <c r="AS4" t="inlineStr">
         <is>
-          <t>Outsourcing transcription services can provide businesses with a cost effective and efficient solution. Rather than having to hire and train personnel, transcription services can be outsourced to provide a quality service with minimal risk. Transcription services are both accurate and professional, offering a high degree of satisfaction for businesses looking to outsource.
-Transcription services are perfect for taking care of customer documents, providing fast and accurate transcriptions. Any important meetings can be stored securely in databases, allowing for easy access at a later date. This can be hugely beneficial for businesses, as it ensures that all conversations and documents are properly managed.
-Conference calls are regularly held in business and transcription services can be used to capture these conversations. Normally, it is difficult to access these recordings, but with the help of transcription services, it doesn’t have to be. Businesses can use the services to record and store their conversations, ensuring that all of the key information is securely stored.
-Interviews can be used for both professional and personal reasons. Transcription services can make sure that the conversation is accurately recorded, meaning that it can be used as ready material in the future. This is more efficient than attempting to do it yourself, as it can take longer to get back into the transcription process.
-Investment transcription is another area where transcription services can be used. This is the process of translating an audio or video file into a written document. This is not a translation service, as it is generally done quickly and accurately. It is often used when footage is recorded in a professional or financial setting, such as in a negotiation. With these transactions, it is important to get accurate and legible transcripts to use as collateral.
-When looking for transcription services, it is important to find a reputable service provider. It is vital to make sure that the service is secure, as data security is always a concern when working with an outside organization. Consider using Catholic Transcription Services to ensure a 100% confidential environment.
-In conclusion, outsourcing transcription services provides businesses with a cost effective and efficient way to manage and store conversations and documents. The services can be used in a range of different ways, from conference calls to interviews and investments. When looking for a transcription service, it is important to make sure that the provider is secure and reliable.</t>
+          <t>Outsourcing transcription services is a great way to save time and money while ensuring accuracy and speed. With the right transcription company, you can enjoy a variety of services such as legal transcription, business transcription, medical transcription, podcast transcription, educational transcription, and more. Plus, modern transcription companies are investing in the latest technologies to provide superior quality and fast turnaround times. 
+Successfully taking advantage of these technological advances requires you to outsource your business transcription needs to a quality transcription firm. Doing this will allow you to leverage their technologies to accomplish your online data collection, which can help you gain competitive advantages and increase the efficiency of your operations. 
+It is important to take the necessary steps to ensure that sensitive information is not compromised when transcribing audio recordings. Doing so starts with selecting the right transcription services provider and setting up a process with checks and balances. Installing transcription software or hiring professionals will likely require you to invest money and time in training, so outsourcing transcription services is a great way to reduce production cost. Transcription companies have the tools and technology to accurately and quickly transcribe your recordings or audio files. 
+Overall, outsourcing transcription services has a variety of benefits that your business can enjoy. Not only does it help reduce production cost, but it also ensures accuracy and quick transcription services. With the right transcription company, you can leverage the latest technologies to get fast and accurate results. Plus, you can rest assured that your sensitive information is secure as long as you take the necessary steps to ensure that this is the case.</t>
         </is>
       </c>
     </row>

</xml_diff>